<commit_message>
renamed operator to blocs, added blocs, made graphs of blocs to simulate a bath
</commit_message>
<xml_diff>
--- a/OpsRoadMap.xlsx
+++ b/OpsRoadMap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swanb\computeGraph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swanb\simulpynk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1957E1FD-9F70-4169-BD24-5283ADD2126D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7330325-4AAF-48C6-8699-AF4DF20F9EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{EBBA4F1F-FD45-4DE7-B3C1-6B25F76701BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="487">
   <si>
     <t>Delay</t>
   </si>
@@ -1485,6 +1485,15 @@
   </si>
   <si>
     <t>See Variable integer Delay</t>
+  </si>
+  <si>
+    <t>See Compare to constant</t>
+  </si>
+  <si>
+    <t>See Linear</t>
+  </si>
+  <si>
+    <t>see Linear</t>
   </si>
 </sst>
 </file>
@@ -1855,8 +1864,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2702,7 @@
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>144</v>
@@ -2979,7 +2988,7 @@
     </row>
     <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>195</v>
@@ -3045,7 +3054,7 @@
     </row>
     <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>207</v>

</xml_diff>